<commit_message>
BTC data corrected to receive datafeed
</commit_message>
<xml_diff>
--- a/DailyTradingPlan.xlsx
+++ b/DailyTradingPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\ibbot100_data\MTA_GitHub\241005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EFC2C1-BE59-4FAD-900F-6259BDABA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB12CC-C92C-4781-A479-F58A620C2F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,7 +670,7 @@
   <dimension ref="A1:CA290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>